<commit_message>
the knn model is tested with different five different data-set (the heightes accuracy is %75)
</commit_message>
<xml_diff>
--- a/Dataset_Test_Eren/Graphs/Results.xlsx
+++ b/Dataset_Test_Eren/Graphs/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\Graduation_Project\Dataset_Test_Eren\Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BB47AC-C91B-42B8-BAF8-04DC9C9CBAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C81F8C6-CED0-4CF6-8432-363981F36094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Dosya Türü</t>
   </si>
@@ -128,6 +128,95 @@
     <t>[[5 2 1]
  [6 1 1]
  [2 2 3]]</t>
+  </si>
+  <si>
+    <t>Dataset_Vector_TopSelected_5.csv</t>
+  </si>
+  <si>
+    <t>Value Mean
+Saturation Mean, Saturation Std
+Skewness a*, Skewness b* (Article)</t>
+  </si>
+  <si>
+    <t>[[4 2 2]
+ [3 4 1]
+ [1 0 6]]</t>
+  </si>
+  <si>
+    <t>[[5 1 2]
+ [3 3 2]
+ [1 0 6]]</t>
+  </si>
+  <si>
+    <t>Dataset_Vector_TopSelected_7.csv</t>
+  </si>
+  <si>
+    <t>Value Mean, Value Std
+Saturation Mean, Saturation Std
+Skewness a*, Skewness b* (Article)
+Hue Mean</t>
+  </si>
+  <si>
+    <t>[[4 3 1]
+ [3 4 1]
+ [0 0 7]]</t>
+  </si>
+  <si>
+    <t>[[6 0 2]
+ [3 5 0]
+ [1 0 6]]</t>
+  </si>
+  <si>
+    <t>Dataset_Vector_TopSelected_6.csv</t>
+  </si>
+  <si>
+    <t>[[5 1 2]
+ [2 5 1]
+ [2 0 5]]</t>
+  </si>
+  <si>
+    <t>Value Mean
+Saturation Mean, Saturation Std
+Skewness a*, Skewness b* (Article)
+Hue Mean</t>
+  </si>
+  <si>
+    <t>Dataset_Vector_TopSelected_4.csv</t>
+  </si>
+  <si>
+    <t>[[4 1 3]
+ [2 5 1]
+ [1 1 5]]</t>
+  </si>
+  <si>
+    <t>[[4 2 2]
+ [3 4 1]
+ [2 1 4]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Value Mean
+Saturation Std,
+Skewness a*, Skewness b* (Article)
+</t>
+  </si>
+  <si>
+    <t>Dataset_Vector_TopSelected_3.csv</t>
+  </si>
+  <si>
+    <t>[[4 1 3]
+ [2 6 0]
+ [1 4 2]]</t>
+  </si>
+  <si>
+    <t>[[4 1 3]
+ [1 6 1]
+ [1 4 2]]</t>
+  </si>
+  <si>
+    <t>Value Mean
+Saturation Std,
+Skewness a* (Article)</t>
   </si>
 </sst>
 </file>
@@ -143,7 +232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +275,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA6CE2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -199,32 +318,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -232,6 +357,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -240,6 +389,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFA6CE2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -514,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I21"/>
+  <dimension ref="B1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,287 +712,599 @@
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="8">
         <v>0.43</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="8">
         <v>0.47</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="8">
         <v>0.61</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="8">
         <v>0.51</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="2:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="10">
         <v>0.48</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="10">
         <v>0.51</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="10">
         <v>0.56999999999999995</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="10">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <v>0.52</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="6">
         <v>0.43</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="6">
         <v>0.65</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="6">
         <v>0.52</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="2:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="4">
         <v>0.48</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="4">
         <v>0.44</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="4">
         <v>0.56999999999999995</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="4">
         <v>0.49</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="12">
         <v>0.39</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="12">
         <v>0.43</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="12">
         <v>0.39</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="12">
         <v>0.41</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="14">
+        <v>0.65</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="14">
+        <v>0.53</v>
+      </c>
+      <c r="G26" s="14">
+        <v>0.74</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="14">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="29" spans="2:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B30" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="16">
+        <v>0.61</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="16">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G30" s="16">
+        <v>0.65</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="16">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+    </row>
+    <row r="33" spans="2:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="18">
+        <v>0.52</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" s="18">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G34" s="18">
+        <v>0.61</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I34" s="18">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+    </row>
+    <row r="37" spans="2:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="20">
+        <v>0.52</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" s="20">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G38" s="20">
+        <v>0.52</v>
+      </c>
+      <c r="H38" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38" s="20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="80">
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="I34:I37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="F38:F41"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="H38:H41"/>
+    <mergeCell ref="I38:I41"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="I26:I29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="I30:I33"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="F26:F29"/>
     <mergeCell ref="G18:G21"/>
     <mergeCell ref="H18:H21"/>
     <mergeCell ref="I18:I21"/>
@@ -873,12 +1339,20 @@
     <mergeCell ref="I10:I13"/>
     <mergeCell ref="H14:H17"/>
     <mergeCell ref="I14:I17"/>
+    <mergeCell ref="G14:G17"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C14:C17"/>
     <mergeCell ref="D14:D17"/>
     <mergeCell ref="E14:E17"/>
     <mergeCell ref="F14:F17"/>
-    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="I22:I25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="F22:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>